<commit_message>
Added new rows on he excel
</commit_message>
<xml_diff>
--- a/Requests/Requests.xlsx
+++ b/Requests/Requests.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PKIPOSMET\Desktop\RPA\RPACapstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PKIPOSMET\Desktop\RPA\RPACapstone\Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D24C0CD-5744-4AD6-B3E1-71C173296109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB14062B-46A1-4D05-9A16-EF4666641863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DayOne" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Contact Name</t>
   </si>
@@ -42,7 +42,16 @@
     <t>Subject</t>
   </si>
   <si>
-    <t>registration assistance</t>
+    <t>Registration assistance</t>
+  </si>
+  <si>
+    <t>Account Name</t>
+  </si>
+  <si>
+    <t>Patrick B</t>
+  </si>
+  <si>
+    <t>Phone</t>
   </si>
 </sst>
 </file>
@@ -87,9 +96,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -371,14 +381,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -404,6 +415,22 @@
       </c>
       <c r="B3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2">
+        <v>728030696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extracted data to excel
</commit_message>
<xml_diff>
--- a/Requests/Requests.xlsx
+++ b/Requests/Requests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PKIPOSMET\Desktop\RPA\RPACapstone\Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB14062B-46A1-4D05-9A16-EF4666641863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66813F75-C91D-4002-A205-5985C14CC5F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,28 +30,28 @@
     <t>Contact Name</t>
   </si>
   <si>
-    <t>Moringa School</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
-    <t>contact@moringaschool.com</t>
-  </si>
-  <si>
     <t>Subject</t>
   </si>
   <si>
-    <t>Registration assistance</t>
-  </si>
-  <si>
     <t>Account Name</t>
   </si>
   <si>
-    <t>Patrick B</t>
-  </si>
-  <si>
     <t>Phone</t>
+  </si>
+  <si>
+    <t>Moringa</t>
+  </si>
+  <si>
+    <t>moringa@email.com</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>Patrick</t>
   </si>
 </sst>
 </file>
@@ -98,8 +98,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -384,7 +384,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -398,39 +398,39 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2">
-        <v>728030696</v>
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>713636981</v>
       </c>
     </row>
   </sheetData>

</xml_diff>